<commit_message>
BeaconConfig app: add advertising-on-motion
Added the possibility of configuring the advertising-on-motion feature on BlueUp beacons with the BeaconConfig app
</commit_message>
<xml_diff>
--- a/BeaconConfigApp/config_file/config_file.xlsx
+++ b/BeaconConfigApp/config_file/config_file.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\workspaces\GIT\CLIMB\sco.climb.driverapp\BeaconConfigApp\config_file\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B766B1F4-3647-42BA-9F2E-704A9B8C2395}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" xr2:uid="{28E8232F-34BB-4B65-A49D-12068765B558}"/>
   </bookViews>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
   <si>
     <t>NAME*</t>
   </si>
@@ -93,6 +94,9 @@
   </si>
   <si>
     <t>00000000000000000000000100000003</t>
+  </si>
+  <si>
+    <t>accel config</t>
   </si>
 </sst>
 </file>
@@ -458,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A05BD5-E542-4C83-9A5A-A7E686461E91}">
-  <dimension ref="A1:T37"/>
+  <dimension ref="A1:U37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,7 +491,7 @@
     <col min="20" max="20" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
@@ -513,7 +517,7 @@
       <c r="S1" s="4"/>
       <c r="T1" s="4"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -574,8 +578,11 @@
       <c r="T2" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="U2" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -606,8 +613,11 @@
       <c r="K3" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="U3">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -638,8 +648,11 @@
       <c r="K4" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="U4">
+        <v>4</v>
+      </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -669,6 +682,9 @@
       </c>
       <c r="K5" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="U5">
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">

</xml_diff>